<commit_message>
add cu content to sodium batteries
</commit_message>
<xml_diff>
--- a/Data/Demand Model/Mineral_Intensity.xlsx
+++ b/Data/Demand Model/Mineral_Intensity.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Pablo\Educacion\Aprendizaje Continuo\Codigos utiles\R\Proyectos R\Critical-Minerals-EV\Data\Demand Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5500F6DE-407D-4207-870A-2CC5B548D2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCEFDFB-D7F5-4E9C-A4EC-609D25BD276E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{3B472435-57B0-4E18-8E2C-2EA77018F632}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B472435-57B0-4E18-8E2C-2EA77018F632}"/>
   </bookViews>
   <sheets>
     <sheet name="BatPac" sheetId="3" r:id="rId1"/>
     <sheet name="Notes" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BatPac!$A$1:$C$206</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BatPac!$A$1:$C$211</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="65">
   <si>
     <t>LFP</t>
   </si>
@@ -177,9 +177,6 @@
     <t xml:space="preserve">Source: </t>
   </si>
   <si>
-    <t>BatPac</t>
-  </si>
-  <si>
     <t xml:space="preserve">Solid state (SS). </t>
   </si>
   <si>
@@ -229,6 +226,15 @@
   </si>
   <si>
     <t>Battery_MWh</t>
+  </si>
+  <si>
+    <t>BatPac 5.1</t>
+  </si>
+  <si>
+    <t>Copper is not on the cathode, but on the negative foil material. SolidPac assumes the same thickness (1o um) as BatPac, so the mineral intensity for copper is assumed to be the same.</t>
+  </si>
+  <si>
+    <t>Copper: Cathode content (based on stochoimetry) + negative material foil content (assume the same as LFP in BatPac)</t>
   </si>
 </sst>
 </file>
@@ -597,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14971A9-44D0-4518-9090-F0BD7475C020}">
-  <dimension ref="A1:C227"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +795,7 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1">
         <v>0.1650656125169381</v>
@@ -1020,7 +1026,7 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="1">
         <v>0.66382364337201216</v>
@@ -1251,7 +1257,7 @@
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C59" s="1">
         <v>0.12499712112480743</v>
@@ -1482,7 +1488,7 @@
         <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C80" s="1">
         <v>0</v>
@@ -1713,7 +1719,7 @@
         <v>12</v>
       </c>
       <c r="B101" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C101" s="1">
         <v>0</v>
@@ -1765,13 +1771,13 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B106" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C106" s="1">
-        <v>0.59497617875035491</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1779,7 +1785,7 @@
         <v>10</v>
       </c>
       <c r="B107" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C107" s="1">
         <v>0.59497617875035491</v>
@@ -1790,10 +1796,10 @@
         <v>10</v>
       </c>
       <c r="B108" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C108" s="1">
-        <v>0.57498279276200925</v>
+        <v>0.59497617875035491</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1801,7 +1807,7 @@
         <v>10</v>
       </c>
       <c r="B109" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C109" s="1">
         <v>0.57498279276200925</v>
@@ -1812,10 +1818,10 @@
         <v>10</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C110" s="1">
-        <v>0.57189011139885271</v>
+        <v>0.57498279276200925</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -1823,7 +1829,7 @@
         <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C111" s="1">
         <v>0.57189011139885271</v>
@@ -1834,10 +1840,10 @@
         <v>10</v>
       </c>
       <c r="B112" t="s">
-        <v>22</v>
-      </c>
-      <c r="C112">
-        <v>0.55501253419738494</v>
+        <v>28</v>
+      </c>
+      <c r="C112" s="1">
+        <v>0.57189011139885271</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -1845,7 +1851,7 @@
         <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C113">
         <v>0.55501253419738494</v>
@@ -1856,9 +1862,9 @@
         <v>10</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" s="1">
+        <v>29</v>
+      </c>
+      <c r="C114">
         <v>0.55501253419738494</v>
       </c>
     </row>
@@ -1867,7 +1873,7 @@
         <v>10</v>
       </c>
       <c r="B115" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C115" s="1">
         <v>0.55501253419738494</v>
@@ -1878,10 +1884,10 @@
         <v>10</v>
       </c>
       <c r="B116" t="s">
-        <v>23</v>
-      </c>
-      <c r="C116">
-        <v>0.57867860601187082</v>
+        <v>30</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0.55501253419738494</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -1889,7 +1895,7 @@
         <v>10</v>
       </c>
       <c r="B117" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C117">
         <v>0.57867860601187082</v>
@@ -1900,10 +1906,10 @@
         <v>10</v>
       </c>
       <c r="B118" t="s">
-        <v>17</v>
-      </c>
-      <c r="C118" s="1">
-        <v>0.5480935387976984</v>
+        <v>32</v>
+      </c>
+      <c r="C118">
+        <v>0.57867860601187082</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -1911,7 +1917,7 @@
         <v>10</v>
       </c>
       <c r="B119" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C119" s="1">
         <v>0.5480935387976984</v>
@@ -1922,10 +1928,10 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C120" s="1">
-        <v>0.56293127178373448</v>
+        <v>0.5480935387976984</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -1933,7 +1939,7 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="C121" s="1">
         <v>0.56293127178373448</v>
@@ -1944,10 +1950,10 @@
         <v>10</v>
       </c>
       <c r="B122" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="C122" s="1">
-        <v>0.72460281058567555</v>
+        <v>0.56293127178373448</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -1955,10 +1961,10 @@
         <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C123" s="1">
-        <v>0.68976796903425919</v>
+        <v>0.72460281058567599</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -1966,10 +1972,10 @@
         <v>10</v>
       </c>
       <c r="B124" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C124" s="1">
-        <v>1.2355941558363768</v>
+        <v>0.68976796903425919</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -1977,32 +1983,32 @@
         <v>10</v>
       </c>
       <c r="B125" t="s">
-        <v>24</v>
-      </c>
-      <c r="C125">
-        <v>0.68976796903425919</v>
+        <v>18</v>
+      </c>
+      <c r="C125" s="1">
+        <v>1.2355941558363768</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B126" t="s">
-        <v>3</v>
-      </c>
-      <c r="C126" s="1">
-        <v>0.41313800625452174</v>
+        <v>24</v>
+      </c>
+      <c r="C126">
+        <v>0.68976796903425919</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B127" t="s">
-        <v>26</v>
-      </c>
-      <c r="C127" s="1">
-        <v>0.41313800625452174</v>
+        <v>42</v>
+      </c>
+      <c r="C127">
+        <v>0.72460281058567599</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -2010,10 +2016,10 @@
         <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C128" s="1">
-        <v>0.3918553123211263</v>
+        <v>0.41313800625452174</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -2021,10 +2027,10 @@
         <v>11</v>
       </c>
       <c r="B129" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C129" s="1">
-        <v>0.3918553123211263</v>
+        <v>0.41313800625452174</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -2032,10 +2038,10 @@
         <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C130" s="1">
-        <v>0.38838216513235024</v>
+        <v>0.3918553123211263</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2043,10 +2049,10 @@
         <v>11</v>
       </c>
       <c r="B131" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C131" s="1">
-        <v>0.38838216513235024</v>
+        <v>0.3918553123211263</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2054,10 +2060,10 @@
         <v>11</v>
       </c>
       <c r="B132" t="s">
-        <v>22</v>
-      </c>
-      <c r="C132">
-        <v>0.36951139005120265</v>
+        <v>4</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0.38838216513235024</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -2065,10 +2071,10 @@
         <v>11</v>
       </c>
       <c r="B133" t="s">
-        <v>29</v>
-      </c>
-      <c r="C133">
-        <v>0.36951139005120265</v>
+        <v>28</v>
+      </c>
+      <c r="C133" s="1">
+        <v>0.38838216513235024</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -2076,9 +2082,9 @@
         <v>11</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
-      </c>
-      <c r="C134" s="1">
+        <v>22</v>
+      </c>
+      <c r="C134">
         <v>0.36951139005120265</v>
       </c>
     </row>
@@ -2087,9 +2093,9 @@
         <v>11</v>
       </c>
       <c r="B135" t="s">
-        <v>30</v>
-      </c>
-      <c r="C135" s="1">
+        <v>29</v>
+      </c>
+      <c r="C135">
         <v>0.36951139005120265</v>
       </c>
     </row>
@@ -2098,9 +2104,9 @@
         <v>11</v>
       </c>
       <c r="B136" t="s">
-        <v>23</v>
-      </c>
-      <c r="C136">
+        <v>5</v>
+      </c>
+      <c r="C136" s="1">
         <v>0.36951139005120265</v>
       </c>
     </row>
@@ -2109,9 +2115,9 @@
         <v>11</v>
       </c>
       <c r="B137" t="s">
-        <v>32</v>
-      </c>
-      <c r="C137">
+        <v>30</v>
+      </c>
+      <c r="C137" s="1">
         <v>0.36951139005120265</v>
       </c>
     </row>
@@ -2120,10 +2126,10 @@
         <v>11</v>
       </c>
       <c r="B138" t="s">
-        <v>17</v>
-      </c>
-      <c r="C138" s="1">
-        <v>0.36094066665892766</v>
+        <v>23</v>
+      </c>
+      <c r="C138">
+        <v>0.36951139005120265</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,10 +2137,10 @@
         <v>11</v>
       </c>
       <c r="B139" t="s">
-        <v>31</v>
-      </c>
-      <c r="C139" s="1">
-        <v>0.36094066665892766</v>
+        <v>32</v>
+      </c>
+      <c r="C139">
+        <v>0.36951139005120265</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,10 +2148,10 @@
         <v>11</v>
       </c>
       <c r="B140" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C140" s="1">
-        <v>0.37760615505433981</v>
+        <v>0.36094066665892766</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -2153,10 +2159,10 @@
         <v>11</v>
       </c>
       <c r="B141" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C141" s="1">
-        <v>0.37760615505433981</v>
+        <v>0.36094066665892766</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,10 +2170,10 @@
         <v>11</v>
       </c>
       <c r="B142" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C142" s="1">
-        <v>0.55106817416551224</v>
+        <v>0.37760615505433981</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,10 +2181,10 @@
         <v>11</v>
       </c>
       <c r="B143" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C143" s="1">
-        <v>0.51908142796905032</v>
+        <v>0.37760615505433981</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2186,10 +2192,10 @@
         <v>11</v>
       </c>
       <c r="B144" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C144" s="1">
-        <v>0.18040752824129977</v>
+        <v>0.55106817416551201</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -2197,43 +2203,44 @@
         <v>11</v>
       </c>
       <c r="B145" t="s">
-        <v>24</v>
-      </c>
-      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="C145" s="1">
         <v>0.51908142796905032</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B146" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C146" s="1">
-        <v>0.97256653113918967</v>
+        <v>0.18040752824129977</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B147" t="s">
-        <v>26</v>
-      </c>
-      <c r="C147" s="1">
-        <v>0.97256653113918967</v>
+        <v>24</v>
+      </c>
+      <c r="C147">
+        <v>0.51908142796905032</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B148" t="s">
-        <v>16</v>
-      </c>
-      <c r="C148" s="1">
-        <v>0.95653132023005516</v>
+        <v>42</v>
+      </c>
+      <c r="C148">
+        <f>0.551068174165512+0.372442155851388</f>
+        <v>0.92351033001690008</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -2241,10 +2248,10 @@
         <v>19</v>
       </c>
       <c r="B149" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C149" s="1">
-        <v>0.95653132023005516</v>
+        <v>0.97256653113918967</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -2252,10 +2259,10 @@
         <v>19</v>
       </c>
       <c r="B150" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C150" s="1">
-        <v>0.95433710505717206</v>
+        <v>0.97256653113918967</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -2263,10 +2270,10 @@
         <v>19</v>
       </c>
       <c r="B151" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C151" s="1">
-        <v>0.95433710505717206</v>
+        <v>0.95653132023005516</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,10 +2281,10 @@
         <v>19</v>
       </c>
       <c r="B152" t="s">
-        <v>22</v>
-      </c>
-      <c r="C152">
-        <v>0.94224070632218504</v>
+        <v>27</v>
+      </c>
+      <c r="C152" s="1">
+        <v>0.95653132023005516</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -2285,10 +2292,10 @@
         <v>19</v>
       </c>
       <c r="B153" t="s">
-        <v>29</v>
-      </c>
-      <c r="C153">
-        <v>0.94224070632218504</v>
+        <v>4</v>
+      </c>
+      <c r="C153" s="1">
+        <v>0.95433710505717206</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -2296,10 +2303,10 @@
         <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C154" s="1">
-        <v>0.94224070632218504</v>
+        <v>0.95433710505717206</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -2307,9 +2314,9 @@
         <v>19</v>
       </c>
       <c r="B155" t="s">
-        <v>30</v>
-      </c>
-      <c r="C155" s="1">
+        <v>22</v>
+      </c>
+      <c r="C155">
         <v>0.94224070632218504</v>
       </c>
     </row>
@@ -2318,7 +2325,7 @@
         <v>19</v>
       </c>
       <c r="B156" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C156">
         <v>0.94224070632218504</v>
@@ -2329,9 +2336,9 @@
         <v>19</v>
       </c>
       <c r="B157" t="s">
-        <v>32</v>
-      </c>
-      <c r="C157">
+        <v>5</v>
+      </c>
+      <c r="C157" s="1">
         <v>0.94224070632218504</v>
       </c>
     </row>
@@ -2340,10 +2347,10 @@
         <v>19</v>
       </c>
       <c r="B158" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C158" s="1">
-        <v>0.93859797599403971</v>
+        <v>0.94224070632218504</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -2351,10 +2358,10 @@
         <v>19</v>
       </c>
       <c r="B159" t="s">
-        <v>31</v>
-      </c>
-      <c r="C159" s="1">
-        <v>0.93859797599403971</v>
+        <v>23</v>
+      </c>
+      <c r="C159">
+        <v>0.94224070632218504</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -2362,10 +2369,10 @@
         <v>19</v>
       </c>
       <c r="B160" t="s">
-        <v>2</v>
-      </c>
-      <c r="C160" s="1">
-        <v>0.94910557779586113</v>
+        <v>32</v>
+      </c>
+      <c r="C160">
+        <v>0.94224070632218504</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2373,10 +2380,10 @@
         <v>19</v>
       </c>
       <c r="B161" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="C161" s="1">
-        <v>0.94910557779586113</v>
+        <v>0.93859797599403971</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -2384,10 +2391,10 @@
         <v>19</v>
       </c>
       <c r="B162" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C162" s="1">
-        <v>1.0773872995285019</v>
+        <v>0.93859797599403971</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -2395,10 +2402,10 @@
         <v>19</v>
       </c>
       <c r="B163" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C163" s="1">
-        <v>1.0406805924516742</v>
+        <v>0.94910557779586113</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -2406,10 +2413,10 @@
         <v>19</v>
       </c>
       <c r="B164" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="C164" s="1">
-        <v>1.3045305828970397</v>
+        <v>0.94910557779586113</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -2417,54 +2424,54 @@
         <v>19</v>
       </c>
       <c r="B165" t="s">
-        <v>24</v>
-      </c>
-      <c r="C165">
-        <v>1.0406805924516742</v>
+        <v>0</v>
+      </c>
+      <c r="C165" s="1">
+        <v>1.0773872995285001</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B166" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C166" s="1">
-        <v>0.35844368109873176</v>
+        <v>1.0406805924516742</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B167" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C167" s="1">
-        <v>0.35844368109873176</v>
+        <v>1.3045305828970397</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B168" t="s">
-        <v>16</v>
-      </c>
-      <c r="C168" s="1">
-        <v>0.35035144896604281</v>
+        <v>24</v>
+      </c>
+      <c r="C168">
+        <v>1.0406805924516742</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B169" t="s">
-        <v>27</v>
-      </c>
-      <c r="C169" s="1">
-        <v>0.35035144896604281</v>
+        <v>42</v>
+      </c>
+      <c r="C169">
+        <v>1.0773872995285001</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -2472,10 +2479,10 @@
         <v>20</v>
       </c>
       <c r="B170" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C170" s="1">
-        <v>0.34922511486496305</v>
+        <v>0.35844368109873176</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -2483,10 +2490,10 @@
         <v>20</v>
       </c>
       <c r="B171" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C171" s="1">
-        <v>0.34922511486496305</v>
+        <v>0.35844368109873176</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2494,10 +2501,10 @@
         <v>20</v>
       </c>
       <c r="B172" t="s">
-        <v>22</v>
-      </c>
-      <c r="C172">
-        <v>0.34299753067970795</v>
+        <v>16</v>
+      </c>
+      <c r="C172" s="1">
+        <v>0.35035144896604281</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -2505,10 +2512,10 @@
         <v>20</v>
       </c>
       <c r="B173" t="s">
-        <v>29</v>
-      </c>
-      <c r="C173">
-        <v>0.34299753067970795</v>
+        <v>27</v>
+      </c>
+      <c r="C173" s="1">
+        <v>0.35035144896604281</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -2516,10 +2523,10 @@
         <v>20</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C174" s="1">
-        <v>0.34299753067970795</v>
+        <v>0.34922511486496305</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -2527,10 +2534,10 @@
         <v>20</v>
       </c>
       <c r="B175" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C175" s="1">
-        <v>0.34299753067970795</v>
+        <v>0.34922511486496305</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -2538,7 +2545,7 @@
         <v>20</v>
       </c>
       <c r="B176" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C176">
         <v>0.34299753067970795</v>
@@ -2549,7 +2556,7 @@
         <v>20</v>
       </c>
       <c r="B177" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C177">
         <v>0.34299753067970795</v>
@@ -2560,10 +2567,10 @@
         <v>20</v>
       </c>
       <c r="B178" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C178" s="1">
-        <v>0.34101017222573737</v>
+        <v>0.34299753067970795</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -2571,10 +2578,10 @@
         <v>20</v>
       </c>
       <c r="B179" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C179" s="1">
-        <v>0.34101017222573737</v>
+        <v>0.34299753067970795</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -2582,10 +2589,10 @@
         <v>20</v>
       </c>
       <c r="B180" t="s">
-        <v>2</v>
-      </c>
-      <c r="C180" s="1">
-        <v>0.34645572810481684</v>
+        <v>23</v>
+      </c>
+      <c r="C180">
+        <v>0.34299753067970795</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -2593,10 +2600,10 @@
         <v>20</v>
       </c>
       <c r="B181" t="s">
-        <v>60</v>
-      </c>
-      <c r="C181" s="1">
-        <v>0.34645572810481684</v>
+        <v>32</v>
+      </c>
+      <c r="C181">
+        <v>0.34299753067970795</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2604,10 +2611,10 @@
         <v>20</v>
       </c>
       <c r="B182" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C182" s="1">
-        <v>0.41071849600216381</v>
+        <v>0.34101017222573737</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -2615,10 +2622,10 @@
         <v>20</v>
       </c>
       <c r="B183" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C183" s="1">
-        <v>0.39276963564934558</v>
+        <v>0.34101017222573737</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -2626,10 +2633,10 @@
         <v>20</v>
       </c>
       <c r="B184" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C184" s="1">
-        <v>0.52202391745442611</v>
+        <v>0.34645572810481684</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -2637,65 +2644,65 @@
         <v>20</v>
       </c>
       <c r="B185" t="s">
-        <v>24</v>
-      </c>
-      <c r="C185">
-        <v>0.39276963564934558</v>
+        <v>59</v>
+      </c>
+      <c r="C185" s="1">
+        <v>0.34645572810481684</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B186" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C186" s="1">
-        <v>0</v>
+        <v>0.41071849600216398</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B187" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C187" s="1">
-        <v>7.830155660747945E-2</v>
+        <v>0.39276963564934558</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B188" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C188" s="1">
-        <v>0</v>
+        <v>0.52202391745442611</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B189" t="s">
-        <v>27</v>
-      </c>
-      <c r="C189" s="1">
-        <v>7.830155660747945E-2</v>
+        <v>24</v>
+      </c>
+      <c r="C189">
+        <v>0.39276963564934558</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B190" t="s">
-        <v>4</v>
-      </c>
-      <c r="C190" s="1">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="C190">
+        <v>0.41071849600216398</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -2703,10 +2710,10 @@
         <v>21</v>
       </c>
       <c r="B191" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C191" s="1">
-        <v>7.7075116651408829E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -2714,10 +2721,10 @@
         <v>21</v>
       </c>
       <c r="B192" t="s">
-        <v>22</v>
-      </c>
-      <c r="C192">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="C192" s="1">
+        <v>7.830155660747945E-2</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -2725,10 +2732,10 @@
         <v>21</v>
       </c>
       <c r="B193" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C193" s="1">
-        <v>7.7075116651408829E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -2736,10 +2743,10 @@
         <v>21</v>
       </c>
       <c r="B194" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C194" s="1">
-        <v>0</v>
+        <v>7.830155660747945E-2</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -2747,10 +2754,10 @@
         <v>21</v>
       </c>
       <c r="B195" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C195" s="1">
-        <v>7.7075116651408829E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -2758,10 +2765,10 @@
         <v>21</v>
       </c>
       <c r="B196" t="s">
-        <v>23</v>
-      </c>
-      <c r="C196">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="C196" s="1">
+        <v>7.7075116651408829E-2</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -2769,10 +2776,10 @@
         <v>21</v>
       </c>
       <c r="B197" t="s">
-        <v>32</v>
-      </c>
-      <c r="C197" s="1">
-        <v>7.7075116651408829E-2</v>
+        <v>22</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -2780,10 +2787,10 @@
         <v>21</v>
       </c>
       <c r="B198" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C198" s="1">
-        <v>0</v>
+        <v>7.7075116651408829E-2</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -2791,10 +2798,10 @@
         <v>21</v>
       </c>
       <c r="B199" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C199" s="1">
-        <v>7.7075116651408829E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -2802,10 +2809,10 @@
         <v>21</v>
       </c>
       <c r="B200" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C200" s="1">
-        <v>0</v>
+        <v>7.7075116651408829E-2</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -2813,10 +2820,10 @@
         <v>21</v>
       </c>
       <c r="B201" t="s">
-        <v>60</v>
-      </c>
-      <c r="C201" s="1">
-        <v>7.8752171663258985E-2</v>
+        <v>23</v>
+      </c>
+      <c r="C201">
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -2824,10 +2831,10 @@
         <v>21</v>
       </c>
       <c r="B202" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C202" s="1">
-        <v>0.39158074976459034</v>
+        <v>7.7075116651408829E-2</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -2835,10 +2842,10 @@
         <v>21</v>
       </c>
       <c r="B203" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C203" s="1">
-        <v>0.12323990834468224</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -2846,10 +2853,10 @@
         <v>21</v>
       </c>
       <c r="B204" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C204" s="1">
-        <v>0</v>
+        <v>7.7075116651408829E-2</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -2857,7 +2864,7 @@
         <v>21</v>
       </c>
       <c r="B205" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C205" s="1">
         <v>0</v>
@@ -2868,73 +2875,73 @@
         <v>21</v>
       </c>
       <c r="B206" t="s">
-        <v>24</v>
-      </c>
-      <c r="C206">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="C206" s="1">
+        <v>7.8752171663258985E-2</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B207" t="s">
-        <v>3</v>
-      </c>
-      <c r="C207" s="4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C207" s="1">
+        <v>0.39158074976459034</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B208" t="s">
-        <v>26</v>
-      </c>
-      <c r="C208" s="4">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="C208" s="1">
+        <v>0.12323990834468224</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B209" t="s">
-        <v>16</v>
-      </c>
-      <c r="C209" s="4">
         <v>1</v>
+      </c>
+      <c r="C209" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B210" t="s">
-        <v>27</v>
-      </c>
-      <c r="C210" s="4">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="C210" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B211" t="s">
-        <v>4</v>
-      </c>
-      <c r="C211" s="4">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="C211">
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B212" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C212" s="4">
         <v>1</v>
@@ -2942,10 +2949,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B213" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C213" s="4">
         <v>1</v>
@@ -2953,10 +2960,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B214" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C214" s="4">
         <v>1</v>
@@ -2964,10 +2971,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B215" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C215" s="4">
         <v>1</v>
@@ -2975,10 +2982,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B216" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C216" s="4">
         <v>1</v>
@@ -2986,10 +2993,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B217" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C217" s="4">
         <v>1</v>
@@ -2997,10 +3004,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B218" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C218" s="4">
         <v>1</v>
@@ -3008,10 +3015,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B219" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C219" s="4">
         <v>1</v>
@@ -3019,10 +3026,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B220" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C220" s="4">
         <v>1</v>
@@ -3030,10 +3037,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B221" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="C221" s="4">
         <v>1</v>
@@ -3041,10 +3048,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B222" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C222" s="4">
         <v>1</v>
@@ -3052,10 +3059,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B223" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C223" s="4">
         <v>1</v>
@@ -3063,10 +3070,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B224" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C224" s="4">
         <v>1</v>
@@ -3074,10 +3081,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B225" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C225" s="4">
         <v>1</v>
@@ -3085,10 +3092,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B226" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C226" s="4">
         <v>1</v>
@@ -3096,17 +3103,72 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B227" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="C227" s="4">
         <v>1</v>
       </c>
     </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>61</v>
+      </c>
+      <c r="B228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C228" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>61</v>
+      </c>
+      <c r="B229" t="s">
+        <v>42</v>
+      </c>
+      <c r="C229" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>61</v>
+      </c>
+      <c r="B230" t="s">
+        <v>1</v>
+      </c>
+      <c r="C230" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>61</v>
+      </c>
+      <c r="B231" t="s">
+        <v>18</v>
+      </c>
+      <c r="C231" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>61</v>
+      </c>
+      <c r="B232" t="s">
+        <v>24</v>
+      </c>
+      <c r="C232" s="4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C206" xr:uid="{D14971A9-44D0-4518-9090-F0BD7475C020}"/>
+  <autoFilter ref="A1:C211" xr:uid="{D14971A9-44D0-4518-9090-F0BD7475C020}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
@@ -3114,10 +3176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF9921A-2AF2-427D-BDE8-40DF7EC99149}">
-  <dimension ref="B1:D23"/>
+  <dimension ref="B1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3127,7 +3189,7 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -3135,28 +3197,28 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
         <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
         <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -3164,15 +3226,15 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
         <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -3185,31 +3247,31 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
         <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -3220,33 +3282,22 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
@@ -3254,23 +3305,44 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix cu in negative foil
</commit_message>
<xml_diff>
--- a/Data/Demand Model/Mineral_Intensity.xlsx
+++ b/Data/Demand Model/Mineral_Intensity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Pablo\Educacion\Aprendizaje Continuo\Codigos utiles\R\Proyectos R\Critical-Minerals-EV\Data\Demand Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCEFDFB-D7F5-4E9C-A4EC-609D25BD276E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D581994-B1F2-4108-912A-5E9CA748F029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B472435-57B0-4E18-8E2C-2EA77018F632}"/>
   </bookViews>
@@ -234,7 +234,7 @@
     <t>Copper is not on the cathode, but on the negative foil material. SolidPac assumes the same thickness (1o um) as BatPac, so the mineral intensity for copper is assumed to be the same.</t>
   </si>
   <si>
-    <t>Copper: Cathode content (based on stochoimetry) + negative material foil content (assume the same as LFP in BatPac)</t>
+    <t>Copper: Cathode content (based on stochoimetry) + content  in terminals (assume results of LFP in BatPac, but using Aluminum as negative foil)</t>
   </si>
 </sst>
 </file>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14971A9-44D0-4518-9090-F0BD7475C020}">
   <dimension ref="A1:C232"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2239,8 +2239,8 @@
         <v>42</v>
       </c>
       <c r="C148">
-        <f>0.551068174165512+0.372442155851388</f>
-        <v>0.92351033001690008</v>
+        <f>0.161501356545118+0.372442155851388</f>
+        <v>0.53394351239650595</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3179,7 +3179,7 @@
   <dimension ref="B1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>